<commit_message>
Updating for Version 2.0 and to allow headspace to have service contacts delivered at an organisation that is at a different PO to the PO that owns the episode.
</commit_message>
<xml_diff>
--- a/data/_orig/headspace-clients-upload.xlsx
+++ b/data/_orig/headspace-clients-upload.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-headspace/data/_orig/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5264A5A9-3B85-5046-947B-FBB7271F0CBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48580" yWindow="4860" windowWidth="25360" windowHeight="15820" activeTab="2"/>
+    <workbookView xWindow="42060" yWindow="3940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="SDQ" sheetId="16" r:id="rId8"/>
     <sheet name="Practitioners" sheetId="17" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="190">
   <si>
     <t>organisation_path</t>
   </si>
@@ -176,9 +182,6 @@
     <t>organisation_state</t>
   </si>
   <si>
-    <t>organisation_status</t>
-  </si>
-  <si>
     <t>organisation_tags</t>
   </si>
   <si>
@@ -188,9 +191,6 @@
     <t>Not for Profit 1</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>CL0001</t>
   </si>
   <si>
@@ -233,12 +233,6 @@
     <t>CL0002-E01</t>
   </si>
   <si>
-    <t>tag3, !nspt</t>
-  </si>
-  <si>
-    <t>!nspt</t>
-  </si>
-  <si>
     <t>service_contact_key</t>
   </si>
   <si>
@@ -590,14 +584,32 @@
     <t>P04</t>
   </si>
   <si>
-    <t>headspace</t>
+    <t>HEADSPACE</t>
+  </si>
+  <si>
+    <t>organisation_start_date</t>
+  </si>
+  <si>
+    <t>organisation_end_date</t>
+  </si>
+  <si>
+    <t>tag3</t>
+  </si>
+  <si>
+    <t>continuity_of_support</t>
+  </si>
+  <si>
+    <t>headspace_funding_source</t>
+  </si>
+  <si>
+    <t>delivery_organisation_path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +629,20 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -652,8 +678,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -670,6 +698,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -957,37 +993,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1001,14 +1037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H1" sqref="H1:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
@@ -1019,7 +1055,7 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,22 +1077,25 @@
       <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
       </c>
       <c r="E2">
         <v>42543098901</v>
@@ -1067,22 +1106,23 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="H2" s="1">
+        <v>1072016</v>
+      </c>
+      <c r="I2" s="1">
+        <v>9099999</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
       </c>
       <c r="E3">
         <v>42543098901</v>
@@ -1093,12 +1133,13 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
+      <c r="H3" s="1">
+        <v>1072016</v>
+      </c>
+      <c r="I3" s="1">
+        <v>9099999</v>
+      </c>
+      <c r="J3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1112,19 +1153,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1159,15 +1200,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>17021983</v>
@@ -1194,15 +1235,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>24092007</v>
@@ -1226,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1240,20 +1281,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1336,18 +1377,21 @@
         <v>36</v>
       </c>
       <c r="AB1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>18062016</v>
@@ -1421,19 +1465,22 @@
       <c r="AA2">
         <v>1</v>
       </c>
-      <c r="AB2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>17072016</v>
@@ -1507,8 +1554,8 @@
       <c r="AA3">
         <v>12</v>
       </c>
-      <c r="AB3" t="s">
-        <v>69</v>
+      <c r="AB3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1522,80 +1569,89 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="18" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>79</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
+        <v>188</v>
+      </c>
+      <c r="R1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="N1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O1" t="s">
-        <v>82</v>
-      </c>
-      <c r="P1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E2">
         <v>21052016</v>
@@ -1633,22 +1689,28 @@
       <c r="P2">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>15062016</v>
@@ -1685,6 +1747,12 @@
       </c>
       <c r="P3">
         <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1698,16 +1766,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1724,63 +1795,66 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>90</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>91</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>92</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>94</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>95</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>96</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>97</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>98</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>100</v>
       </c>
-      <c r="R1" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" t="s">
-        <v>103</v>
-      </c>
-      <c r="U1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>21022016</v>
@@ -1788,61 +1862,64 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>3</v>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
       <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
       <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
         <v>4</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
       <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
         <v>4</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>5</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4</v>
       </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
       <c r="Q2">
         <v>3</v>
       </c>
       <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
         <v>5</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>4</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>10042016</v>
@@ -1850,61 +1927,64 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>3</v>
+      <c r="F3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3">
         <v>4</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
         <v>5</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>4</v>
       </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
       <c r="Q3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S3">
         <v>4</v>
       </c>
       <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>25062016</v>
@@ -1912,32 +1992,32 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>2</v>
+      <c r="F4" t="s">
+        <v>61</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
         <v>4</v>
       </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
       <c r="M4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>4</v>
@@ -1946,27 +2026,30 @@
         <v>4</v>
       </c>
       <c r="Q4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S4">
         <v>2</v>
       </c>
       <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>17072016</v>
@@ -1974,49 +2057,52 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
+      <c r="F5" t="s">
+        <v>61</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
         <v>4</v>
       </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
       <c r="N5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5">
         <v>2</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
         <v>99</v>
       </c>
     </row>
@@ -2031,16 +2117,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2057,36 +2146,39 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
       </c>
-      <c r="I1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>28042016</v>
@@ -2094,37 +2186,40 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>61</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>99</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>18062016</v>
@@ -2132,8 +2227,8 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>9</v>
+      <c r="F3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -2148,21 +2243,24 @@
         <v>9</v>
       </c>
       <c r="K3">
+        <v>9</v>
+      </c>
+      <c r="L3">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>27062016</v>
@@ -2170,34 +2268,37 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>3</v>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
       <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>17062016</v>
@@ -2205,22 +2306,25 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>2</v>
+      <c r="F5" t="s">
+        <v>61</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
       <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
         <v>99</v>
       </c>
     </row>
@@ -2235,16 +2339,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:BE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2261,168 +2368,171 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>122</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>123</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>124</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>125</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>126</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>129</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>131</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>132</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
         <v>133</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>134</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>135</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>136</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>137</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>138</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AF1" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AG1" t="s">
         <v>142</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AH1" t="s">
         <v>143</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>144</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>145</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AL1" t="s">
         <v>147</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>148</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" t="s">
         <v>150</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>151</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>152</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>153</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AS1" t="s">
         <v>154</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AT1" t="s">
         <v>155</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AU1" t="s">
         <v>156</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AV1" t="s">
         <v>157</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AW1" t="s">
         <v>158</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AX1" t="s">
         <v>159</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AY1" t="s">
         <v>160</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AZ1" t="s">
         <v>161</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BA1" t="s">
         <v>162</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BB1" t="s">
         <v>163</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BC1" t="s">
         <v>164</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BD1" t="s">
         <v>165</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BE1" t="s">
         <v>166</v>
       </c>
-      <c r="BA1" t="s">
-        <v>167</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>168</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>169</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:56">
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>15062016</v>
@@ -2431,124 +2541,124 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
       </c>
       <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
       <c r="J2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L2">
+        <v>9</v>
+      </c>
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
       <c r="Q2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
         <v>0</v>
       </c>
-      <c r="W2">
-        <v>2</v>
-      </c>
       <c r="X2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2">
         <v>1</v>
       </c>
       <c r="Z2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
         <v>0</v>
       </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
       <c r="AC2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
         <v>0</v>
       </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
       <c r="AG2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH2">
+        <v>2</v>
+      </c>
+      <c r="AI2">
         <v>0</v>
       </c>
-      <c r="AI2">
-        <v>1</v>
-      </c>
       <c r="AJ2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK2">
+        <v>2</v>
+      </c>
+      <c r="AL2">
         <v>0</v>
       </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
       <c r="AM2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AO2">
         <v>8</v>
       </c>
       <c r="AP2">
+        <v>8</v>
+      </c>
+      <c r="AQ2">
         <v>0</v>
       </c>
-      <c r="AQ2">
-        <v>2</v>
-      </c>
       <c r="AR2">
         <v>2</v>
       </c>
       <c r="AS2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AT2">
         <v>8</v>
@@ -2560,7 +2670,7 @@
         <v>8</v>
       </c>
       <c r="AW2">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="AX2">
         <v>99</v>
@@ -2580,19 +2690,22 @@
       <c r="BC2">
         <v>99</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BD2">
+        <v>99</v>
+      </c>
+      <c r="BE2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:56">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>17062016</v>
@@ -2600,11 +2713,11 @@
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3">
-        <v>9</v>
+      <c r="F3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>170</v>
       </c>
       <c r="H3">
         <v>9</v>
@@ -2682,11 +2795,11 @@
         <v>9</v>
       </c>
       <c r="AG3">
+        <v>9</v>
+      </c>
+      <c r="AH3">
         <v>8</v>
       </c>
-      <c r="AH3">
-        <v>9</v>
-      </c>
       <c r="AI3">
         <v>9</v>
       </c>
@@ -2709,7 +2822,7 @@
         <v>9</v>
       </c>
       <c r="AP3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AQ3">
         <v>8</v>
@@ -2730,36 +2843,39 @@
         <v>8</v>
       </c>
       <c r="AW3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AX3">
         <v>3</v>
       </c>
       <c r="AY3">
+        <v>3</v>
+      </c>
+      <c r="AZ3">
         <v>6</v>
       </c>
-      <c r="AZ3">
-        <v>3</v>
-      </c>
       <c r="BA3">
+        <v>3</v>
+      </c>
+      <c r="BB3">
         <v>8</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>15</v>
       </c>
-      <c r="BC3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56">
+      <c r="BD3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>13062016</v>
@@ -2767,11 +2883,11 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>172</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2792,17 +2908,17 @@
         <v>1</v>
       </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
       <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
       <c r="R4">
         <v>1</v>
       </c>
@@ -2810,19 +2926,19 @@
         <v>1</v>
       </c>
       <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
         <v>0</v>
       </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
       <c r="V4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -2831,25 +2947,25 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
         <v>0</v>
       </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
       <c r="AE4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF4">
+        <v>2</v>
+      </c>
+      <c r="AG4">
         <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>8</v>
       </c>
       <c r="AH4">
         <v>8</v>
@@ -2870,13 +2986,13 @@
         <v>8</v>
       </c>
       <c r="AN4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
       <c r="AP4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AQ4">
         <v>8</v>
@@ -2897,7 +3013,7 @@
         <v>8</v>
       </c>
       <c r="AW4">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="AX4">
         <v>99</v>
@@ -2915,6 +3031,9 @@
         <v>99</v>
       </c>
       <c r="BC4">
+        <v>99</v>
+      </c>
+      <c r="BD4">
         <v>99</v>
       </c>
     </row>
@@ -2929,50 +3048,50 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" t="s">
         <v>177</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>178</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -2996,12 +3115,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3022,15 +3141,15 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -3051,12 +3170,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>99</v>

</xml_diff>

<commit_message>
Updating example upload files.
</commit_message>
<xml_diff>
--- a/data/_orig/headspace-clients-upload.xlsx
+++ b/data/_orig/headspace-clients-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-headspace/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5264A5A9-3B85-5046-947B-FBB7271F0CBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D07E598-BD22-EB42-89CF-EB0B6F973862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42060" yWindow="3940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,10 +599,10 @@
     <t>continuity_of_support</t>
   </si>
   <si>
-    <t>headspace_funding_source</t>
-  </si>
-  <si>
     <t>delivery_organisation_path</t>
+  </si>
+  <si>
+    <t>funding_source</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1573,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R6"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1631,10 +1631,10 @@
         <v>79</v>
       </c>
       <c r="Q1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" t="s">
         <v>188</v>
-      </c>
-      <c r="R1" t="s">
-        <v>189</v>
       </c>
       <c r="S1" t="s">
         <v>80</v>
@@ -1795,7 +1795,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>85</v>
@@ -2146,7 +2146,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>105</v>
@@ -2368,7 +2368,7 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
Moved delivery organisation path to be before practitioner key on service contact.
</commit_message>
<xml_diff>
--- a/data/_orig/headspace-clients-upload.xlsx
+++ b/data/_orig/headspace-clients-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-headspace/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D07E598-BD22-EB42-89CF-EB0B6F973862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E4FF52-4351-7B45-AC25-D8F7887F2CA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42060" yWindow="3940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1572,13 +1572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="18" width="19" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="17" max="18" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -1592,49 +1593,49 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>77</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>78</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>189</v>
-      </c>
-      <c r="R1" t="s">
-        <v>188</v>
       </c>
       <c r="S1" t="s">
         <v>80</v>
@@ -1651,49 +1652,49 @@
         <v>64</v>
       </c>
       <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>82</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>21052016</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>9999</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
@@ -1709,38 +1710,38 @@
       <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>15062016</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>9999</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>5</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -1751,8 +1752,8 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>11</v>
+      <c r="R3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing errors in example upload files.
</commit_message>
<xml_diff>
--- a/data/_orig/headspace-clients-upload.xlsx
+++ b/data/_orig/headspace-clients-upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec-headspace/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E4FF52-4351-7B45-AC25-D8F7887F2CA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF92EE8-23C9-F144-B37D-EF961C8B3D89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42060" yWindow="3940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51000" yWindow="4940" windowWidth="25360" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="190">
   <si>
     <t>organisation_path</t>
   </si>
@@ -1573,11 +1573,12 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="17" max="18" width="19" customWidth="1"/>
   </cols>
@@ -3050,13 +3051,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3195,6 +3201,35 @@
       </c>
       <c r="H5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1973</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>